<commit_message>
made changes to unittests
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -20,7 +20,7 @@
     <t>No. of Images</t>
   </si>
   <si>
-    <t>No. of  CSS</t>
+    <t>No. of CSS</t>
   </si>
   <si>
     <t>Scripts</t>
@@ -115,7 +115,7 @@
   <cols>
     <col min="1" max="1" width="6.96875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.35546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.69140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.1953125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.00390625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="22.5390625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="20.30078125" customWidth="true" bestFit="true"/>

</xml_diff>